<commit_message>
Toán tử so sánh
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/3.thao-tac-voi-cac-nhom-Toan-tu.xlsx
+++ b/1.nen-tang-lap-trinh-java/3.thao-tac-voi-cac-nhom-Toan-tu.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFA9994-3BFD-4287-8586-F6772FC0091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0C935C-C06E-4401-ADEC-962A30C19AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="1050" windowWidth="25215" windowHeight="13650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30405" yWindow="1050" windowWidth="25740" windowHeight="13545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toán tử số học" sheetId="1" r:id="rId1"/>
     <sheet name="Toán tử gán" sheetId="2" r:id="rId2"/>
     <sheet name="Toán tử ++ --" sheetId="3" r:id="rId3"/>
+    <sheet name="Toán tử so sánh" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
   <si>
     <t>java_training</t>
     <phoneticPr fontId="1"/>
@@ -481,6 +482,104 @@
     <t>numberEnd		= --numberStart;</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <r>
+      <t>Toán t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ử</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> so sánh &gt; &lt; &gt;= &lt;= == != &lt;&gt;</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>= numberOne &gt; numberTwo;</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " &gt; " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>= numberOne &gt;= numberTwo;</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " &gt;= " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>= numberOne &lt; numberTwo;</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " &lt; " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>= numberOne &lt;= numberTwo;</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " &lt;= " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>= (numberOne == numberTwo);</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " == " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>= (numberOne != numberTwo);</t>
+  </si>
+  <si>
+    <t>System.out.println(numberOne + " != " + numberTwo + " is " + result);</t>
+  </si>
+  <si>
+    <t>// 003 Toan tu ++ --</t>
+  </si>
+  <si>
+    <t>public static void main003(String[] args) {</t>
+  </si>
+  <si>
+    <t>int numberStart</t>
+  </si>
+  <si>
+    <t>int numberEnd</t>
+  </si>
+  <si>
+    <t>= 0;</t>
+  </si>
+  <si>
+    <t>numberEnd</t>
+  </si>
+  <si>
+    <t>= ++numberStart;</t>
+  </si>
+  <si>
+    <t>= --numberStart;</t>
+  </si>
+  <si>
+    <t>int numberOne		= 3;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int numberTwo		= 5;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>boolean result	= false;</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -637,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -654,7 +753,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -896,6 +994,99 @@
         <a:xfrm>
           <a:off x="809625" y="27755850"/>
           <a:ext cx="10422223" cy="4698413"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>50700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24AA4DE-A6F8-BA4C-0702-535131092AA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="23209250"/>
+          <a:ext cx="12106275" cy="7927875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>145075</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>30878</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F842C1C-A08D-102A-9DE7-1821A05E20B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885825" y="31918275"/>
+          <a:ext cx="7800000" cy="6971428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1172,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N84"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
@@ -1663,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307A0DD8-8EA9-4736-83CE-3F551426B357}">
   <dimension ref="B3:M119"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S105" sqref="S105"/>
     </sheetView>
   </sheetViews>
@@ -2174,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB25F74-AC0D-47DA-A31C-96DACDFC2F7C}">
   <dimension ref="B3:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U130" sqref="U130"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2239,43 +2430,20 @@
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="13" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="13" t="s">
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="11" t="s">
@@ -2307,906 +2475,441 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="4"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="4"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="4"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13" t="s">
+      <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="4"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
+      <c r="D23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="4"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="D24" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="4"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13" t="s">
+      <c r="D25" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="2:12">
       <c r="B26" s="4"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13" t="s">
+      <c r="D26" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" spans="2:12">
       <c r="B27" s="4"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13" t="s">
+      <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="4"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="4"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="4"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
+      <c r="D30" s="12"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="4"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="4"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="2:12">
       <c r="B33" s="4"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="2:12">
       <c r="B34" s="4"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="2:12">
       <c r="B35" s="4"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="2:12">
       <c r="B36" s="4"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="2:12">
       <c r="B37" s="4"/>
-      <c r="C37" s="13" t="s">
+      <c r="C37" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="2:12">
       <c r="B38" s="4"/>
-      <c r="C38" s="13" t="s">
+      <c r="C38" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="2:12">
       <c r="B39" s="4"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13" t="s">
+      <c r="D39" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="2:12">
       <c r="B40" s="4"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="2:12">
       <c r="B41" s="4"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="2:12">
       <c r="B42" s="4"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13" t="s">
+      <c r="D42" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" t="s">
         <v>61</v>
       </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="2:12">
       <c r="B43" s="4"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="13" t="e">
+      <c r="F43" t="e">
         <f xml:space="preserve"> number - 10</f>
         <v>#NAME?</v>
       </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="2:12">
       <c r="B44" s="4"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" t="s">
         <v>63</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="13" t="e">
+      <c r="F44" t="e">
         <f xml:space="preserve"> number * 10</f>
         <v>#NAME?</v>
       </c>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="2:12">
       <c r="B45" s="4"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13" t="s">
+      <c r="D45" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" t="s">
         <v>60</v>
       </c>
-      <c r="F45" s="13" t="e">
+      <c r="F45" t="e">
         <f xml:space="preserve"> number / 10</f>
         <v>#NAME?</v>
       </c>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="2:12">
       <c r="B46" s="4"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13" t="s">
+      <c r="D46" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" t="s">
         <v>60</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="F46" t="s">
         <v>66</v>
       </c>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="2:12">
       <c r="B47" s="4"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13" t="s">
+      <c r="D47" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="2:12">
       <c r="B48" s="4"/>
-      <c r="C48" s="13" t="s">
+      <c r="C48" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="2:12">
       <c r="B49" s="4"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="2:12">
       <c r="B50" s="4"/>
-      <c r="C50" s="13" t="s">
+      <c r="C50" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="2:12">
       <c r="B51" s="4"/>
-      <c r="C51" s="13" t="s">
+      <c r="C51" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="2:12">
       <c r="B52" s="4"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13" t="s">
+      <c r="D52" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="2:12">
       <c r="B53" s="4"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13" t="s">
+      <c r="D53" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="2:12">
       <c r="B54" s="4"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13" t="s">
+      <c r="D54" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="2:12">
       <c r="B55" s="4"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="2:12">
       <c r="B56" s="4"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13" t="s">
+      <c r="D56" t="s">
         <v>16</v>
       </c>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="2:12">
       <c r="B57" s="4"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13" t="s">
+      <c r="D57" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="2:12">
       <c r="B58" s="4"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13" t="s">
+      <c r="D58" t="s">
         <v>19</v>
       </c>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="2:12">
       <c r="B59" s="4"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="2:12">
       <c r="B60" s="4"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13" t="s">
+      <c r="D60" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="2:12">
       <c r="B61" s="4"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13" t="s">
+      <c r="D61" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" t="s">
         <v>21</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="2:12">
       <c r="B62" s="4"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13" t="s">
+      <c r="D62" t="s">
         <v>22</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="2:12">
       <c r="B63" s="4"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="2:12">
       <c r="B64" s="4"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13" t="s">
+      <c r="D64" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="2:12">
       <c r="B65" s="4"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13" t="s">
+      <c r="D65" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="E65" t="s">
         <v>24</v>
       </c>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="2:12">
       <c r="B66" s="4"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13" t="s">
+      <c r="D66" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="2:12">
       <c r="B67" s="4"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="2:12">
       <c r="B68" s="4"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13" t="s">
+      <c r="D68" t="s">
         <v>26</v>
       </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="2:12">
       <c r="B69" s="4"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13" t="s">
+      <c r="D69" t="s">
         <v>27</v>
       </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="2:12">
       <c r="B70" s="4"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13" t="s">
+      <c r="D70" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="E70" t="s">
         <v>28</v>
       </c>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="2:12">
       <c r="B71" s="4"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13" t="s">
+      <c r="D71" t="s">
         <v>29</v>
       </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
       <c r="L71" s="5"/>
     </row>
     <row r="72" spans="2:12">
       <c r="B72" s="4"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
       <c r="L72" s="5"/>
     </row>
     <row r="73" spans="2:12">
       <c r="B73" s="4"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13" t="s">
+      <c r="D73" t="s">
         <v>30</v>
       </c>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="2:12">
       <c r="B74" s="4"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13" t="s">
+      <c r="D74" t="s">
         <v>17</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E74" t="s">
         <v>31</v>
       </c>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="2:12">
       <c r="B75" s="4"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13" t="s">
+      <c r="D75" t="s">
         <v>32</v>
       </c>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
       <c r="L75" s="5"/>
     </row>
     <row r="76" spans="2:12">
       <c r="B76" s="4"/>
-      <c r="C76" s="13" t="s">
+      <c r="C76" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
       <c r="L76" s="5"/>
     </row>
     <row r="77" spans="2:12">
       <c r="B77" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="2:12">
@@ -3245,401 +2948,86 @@
     </row>
     <row r="122" spans="2:18">
       <c r="B122" s="4"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="13"/>
-      <c r="K122" s="13"/>
-      <c r="L122" s="13"/>
-      <c r="M122" s="13"/>
-      <c r="N122" s="13"/>
-      <c r="O122" s="13"/>
-      <c r="P122" s="13"/>
-      <c r="Q122" s="13"/>
       <c r="R122" s="5"/>
     </row>
     <row r="123" spans="2:18">
       <c r="B123" s="4"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="13"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="13"/>
-      <c r="O123" s="13"/>
-      <c r="P123" s="13"/>
-      <c r="Q123" s="13"/>
       <c r="R123" s="5"/>
     </row>
     <row r="124" spans="2:18">
       <c r="B124" s="4"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
-      <c r="M124" s="13"/>
-      <c r="N124" s="13"/>
-      <c r="O124" s="13"/>
-      <c r="P124" s="13"/>
-      <c r="Q124" s="13"/>
       <c r="R124" s="5"/>
     </row>
     <row r="125" spans="2:18">
       <c r="B125" s="4"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="13"/>
-      <c r="M125" s="13"/>
-      <c r="N125" s="13"/>
-      <c r="O125" s="13"/>
-      <c r="P125" s="13"/>
-      <c r="Q125" s="13"/>
       <c r="R125" s="5"/>
     </row>
     <row r="126" spans="2:18">
       <c r="B126" s="4"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
-      <c r="J126" s="13"/>
-      <c r="K126" s="13"/>
-      <c r="L126" s="13"/>
-      <c r="M126" s="13"/>
-      <c r="N126" s="13"/>
-      <c r="O126" s="13"/>
-      <c r="P126" s="13"/>
-      <c r="Q126" s="13"/>
       <c r="R126" s="5"/>
     </row>
     <row r="127" spans="2:18">
       <c r="B127" s="4"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
-      <c r="L127" s="13"/>
-      <c r="M127" s="13"/>
-      <c r="N127" s="13"/>
-      <c r="O127" s="13"/>
-      <c r="P127" s="13"/>
-      <c r="Q127" s="13"/>
       <c r="R127" s="5"/>
     </row>
     <row r="128" spans="2:18">
       <c r="B128" s="4"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-      <c r="L128" s="13"/>
-      <c r="M128" s="13"/>
-      <c r="N128" s="13"/>
-      <c r="O128" s="13"/>
-      <c r="P128" s="13"/>
-      <c r="Q128" s="13"/>
       <c r="R128" s="5"/>
     </row>
     <row r="129" spans="2:18">
       <c r="B129" s="4"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
-      <c r="G129" s="13"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
-      <c r="J129" s="13"/>
-      <c r="K129" s="13"/>
-      <c r="L129" s="13"/>
-      <c r="M129" s="13"/>
-      <c r="N129" s="13"/>
-      <c r="O129" s="13"/>
-      <c r="P129" s="13"/>
-      <c r="Q129" s="13"/>
       <c r="R129" s="5"/>
     </row>
     <row r="130" spans="2:18">
       <c r="B130" s="4"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
-      <c r="G130" s="13"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="13"/>
-      <c r="L130" s="13"/>
-      <c r="M130" s="13"/>
-      <c r="N130" s="13"/>
-      <c r="O130" s="13"/>
-      <c r="P130" s="13"/>
-      <c r="Q130" s="13"/>
       <c r="R130" s="5"/>
     </row>
     <row r="131" spans="2:18">
       <c r="B131" s="4"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="13"/>
-      <c r="M131" s="13"/>
-      <c r="N131" s="13"/>
-      <c r="O131" s="13"/>
-      <c r="P131" s="13"/>
-      <c r="Q131" s="13"/>
       <c r="R131" s="5"/>
     </row>
     <row r="132" spans="2:18">
       <c r="B132" s="4"/>
-      <c r="C132" s="13"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
-      <c r="K132" s="13"/>
-      <c r="L132" s="13"/>
-      <c r="M132" s="13"/>
-      <c r="N132" s="13"/>
-      <c r="O132" s="13"/>
-      <c r="P132" s="13"/>
-      <c r="Q132" s="13"/>
       <c r="R132" s="5"/>
     </row>
     <row r="133" spans="2:18">
       <c r="B133" s="4"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="13"/>
-      <c r="M133" s="13"/>
-      <c r="N133" s="13"/>
-      <c r="O133" s="13"/>
-      <c r="P133" s="13"/>
-      <c r="Q133" s="13"/>
       <c r="R133" s="5"/>
     </row>
     <row r="134" spans="2:18">
       <c r="B134" s="4"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
-      <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
-      <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-      <c r="L134" s="13"/>
-      <c r="M134" s="13"/>
-      <c r="N134" s="13"/>
-      <c r="O134" s="13"/>
-      <c r="P134" s="13"/>
-      <c r="Q134" s="13"/>
       <c r="R134" s="5"/>
     </row>
     <row r="135" spans="2:18">
       <c r="B135" s="4"/>
-      <c r="C135" s="13"/>
-      <c r="D135" s="13"/>
-      <c r="E135" s="13"/>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
-      <c r="L135" s="13"/>
-      <c r="M135" s="13"/>
-      <c r="N135" s="13"/>
-      <c r="O135" s="13"/>
-      <c r="P135" s="13"/>
-      <c r="Q135" s="13"/>
       <c r="R135" s="5"/>
     </row>
     <row r="136" spans="2:18">
       <c r="B136" s="4"/>
-      <c r="C136" s="13"/>
-      <c r="D136" s="13"/>
-      <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
-      <c r="G136" s="13"/>
-      <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
-      <c r="J136" s="13"/>
-      <c r="K136" s="13"/>
-      <c r="L136" s="13"/>
-      <c r="M136" s="13"/>
-      <c r="N136" s="13"/>
-      <c r="O136" s="13"/>
-      <c r="P136" s="13"/>
-      <c r="Q136" s="13"/>
       <c r="R136" s="5"/>
     </row>
     <row r="137" spans="2:18">
       <c r="B137" s="4"/>
-      <c r="C137" s="13"/>
-      <c r="D137" s="13"/>
-      <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
-      <c r="J137" s="13"/>
-      <c r="K137" s="13"/>
-      <c r="L137" s="13"/>
-      <c r="M137" s="13"/>
-      <c r="N137" s="13"/>
-      <c r="O137" s="13"/>
-      <c r="P137" s="13"/>
-      <c r="Q137" s="13"/>
       <c r="R137" s="5"/>
     </row>
     <row r="138" spans="2:18">
       <c r="B138" s="4"/>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
-      <c r="J138" s="13"/>
-      <c r="K138" s="13"/>
-      <c r="L138" s="13"/>
-      <c r="M138" s="13"/>
-      <c r="N138" s="13"/>
-      <c r="O138" s="13"/>
-      <c r="P138" s="13"/>
-      <c r="Q138" s="13"/>
       <c r="R138" s="5"/>
     </row>
     <row r="139" spans="2:18">
       <c r="B139" s="4"/>
-      <c r="C139" s="13"/>
-      <c r="D139" s="13"/>
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
-      <c r="J139" s="13"/>
-      <c r="K139" s="13"/>
-      <c r="L139" s="13"/>
-      <c r="M139" s="13"/>
-      <c r="N139" s="13"/>
-      <c r="O139" s="13"/>
-      <c r="P139" s="13"/>
-      <c r="Q139" s="13"/>
       <c r="R139" s="5"/>
     </row>
     <row r="140" spans="2:18">
       <c r="B140" s="4"/>
-      <c r="C140" s="13"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
-      <c r="J140" s="13"/>
-      <c r="K140" s="13"/>
-      <c r="L140" s="13"/>
-      <c r="M140" s="13"/>
-      <c r="N140" s="13"/>
-      <c r="O140" s="13"/>
-      <c r="P140" s="13"/>
-      <c r="Q140" s="13"/>
       <c r="R140" s="5"/>
     </row>
     <row r="141" spans="2:18">
       <c r="B141" s="4"/>
-      <c r="C141" s="13"/>
-      <c r="D141" s="13"/>
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
-      <c r="J141" s="13"/>
-      <c r="K141" s="13"/>
-      <c r="L141" s="13"/>
-      <c r="M141" s="13"/>
-      <c r="N141" s="13"/>
-      <c r="O141" s="13"/>
-      <c r="P141" s="13"/>
-      <c r="Q141" s="13"/>
       <c r="R141" s="5"/>
     </row>
     <row r="142" spans="2:18">
       <c r="B142" s="4"/>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
-      <c r="K142" s="13"/>
-      <c r="L142" s="13"/>
-      <c r="M142" s="13"/>
-      <c r="N142" s="13"/>
-      <c r="O142" s="13"/>
-      <c r="P142" s="13"/>
-      <c r="Q142" s="13"/>
       <c r="R142" s="5"/>
     </row>
     <row r="143" spans="2:18">
@@ -3666,4 +3054,1986 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57683A45-FCC2-4D7F-9BEA-2FB67D26D9D6}">
+  <dimension ref="B3:N171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="W140" sqref="W140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="4"/>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="4"/>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="4"/>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="4"/>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="4"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="4"/>
+      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="4"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="4"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="4"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="4"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="4"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="B24" s="4"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="4"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="B26" s="4"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="B27" s="4"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="2:13">
+      <c r="B28" s="4"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="B29" s="4"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="B30" s="4"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="2:13">
+      <c r="B31" s="4"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="B32" s="4"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" s="4"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" s="4"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="4"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" s="4"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="4"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="4"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" s="4"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" s="4"/>
+      <c r="C40" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" s="4"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" s="4"/>
+      <c r="C42" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="2:13">
+      <c r="B43" s="4"/>
+      <c r="C43" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" s="4"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="2:13">
+      <c r="B45" s="4"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" spans="2:13">
+      <c r="B46" s="4"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="5"/>
+    </row>
+    <row r="47" spans="2:13">
+      <c r="B47" s="4"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="5"/>
+    </row>
+    <row r="48" spans="2:13">
+      <c r="B48" s="4"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="5"/>
+    </row>
+    <row r="49" spans="2:13">
+      <c r="B49" s="4"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="5"/>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" s="4"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="5"/>
+    </row>
+    <row r="51" spans="2:13">
+      <c r="B51" s="4"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="5"/>
+    </row>
+    <row r="52" spans="2:13">
+      <c r="B52" s="4"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="5"/>
+    </row>
+    <row r="53" spans="2:13">
+      <c r="B53" s="4"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="5"/>
+    </row>
+    <row r="54" spans="2:13">
+      <c r="B54" s="4"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="5"/>
+    </row>
+    <row r="55" spans="2:13">
+      <c r="B55" s="4"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="5"/>
+    </row>
+    <row r="56" spans="2:13">
+      <c r="B56" s="4"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="5"/>
+    </row>
+    <row r="57" spans="2:13">
+      <c r="B57" s="4"/>
+      <c r="C57" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="5"/>
+    </row>
+    <row r="58" spans="2:13">
+      <c r="B58" s="4"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="5"/>
+    </row>
+    <row r="59" spans="2:13">
+      <c r="B59" s="4"/>
+      <c r="C59" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="5"/>
+    </row>
+    <row r="60" spans="2:13">
+      <c r="B60" s="4"/>
+      <c r="C60" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="5"/>
+    </row>
+    <row r="61" spans="2:13">
+      <c r="B61" s="4"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="5"/>
+    </row>
+    <row r="62" spans="2:13">
+      <c r="B62" s="4"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="5"/>
+    </row>
+    <row r="63" spans="2:13">
+      <c r="B63" s="4"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="5"/>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" s="4"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="2:13">
+      <c r="B65" s="4"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F65" s="13" t="e">
+        <f xml:space="preserve"> number - 10</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="2:13">
+      <c r="B66" s="4"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F66" s="13" t="e">
+        <f xml:space="preserve"> number * 10</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="5"/>
+    </row>
+    <row r="67" spans="2:13">
+      <c r="B67" s="4"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F67" s="13" t="e">
+        <f xml:space="preserve"> number / 10</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="5"/>
+    </row>
+    <row r="68" spans="2:13">
+      <c r="B68" s="4"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="5"/>
+    </row>
+    <row r="69" spans="2:13">
+      <c r="B69" s="4"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="5"/>
+    </row>
+    <row r="70" spans="2:13">
+      <c r="B70" s="4"/>
+      <c r="C70" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="5"/>
+    </row>
+    <row r="71" spans="2:13">
+      <c r="B71" s="4"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="5"/>
+    </row>
+    <row r="72" spans="2:13">
+      <c r="B72" s="4"/>
+      <c r="C72" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="5"/>
+    </row>
+    <row r="73" spans="2:13">
+      <c r="B73" s="4"/>
+      <c r="C73" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="5"/>
+    </row>
+    <row r="74" spans="2:13">
+      <c r="B74" s="4"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="5"/>
+    </row>
+    <row r="75" spans="2:13">
+      <c r="B75" s="4"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="2:13">
+      <c r="B76" s="4"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="2:13">
+      <c r="B77" s="4"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="2:13">
+      <c r="B78" s="4"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="2:13">
+      <c r="B79" s="4"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="2:13">
+      <c r="B80" s="4"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="2:13">
+      <c r="B81" s="4"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="2:13">
+      <c r="B82" s="4"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="5"/>
+    </row>
+    <row r="83" spans="2:13">
+      <c r="B83" s="4"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="5"/>
+    </row>
+    <row r="84" spans="2:13">
+      <c r="B84" s="4"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="5"/>
+    </row>
+    <row r="85" spans="2:13">
+      <c r="B85" s="4"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="5"/>
+    </row>
+    <row r="86" spans="2:13">
+      <c r="B86" s="4"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="5"/>
+    </row>
+    <row r="87" spans="2:13">
+      <c r="B87" s="4"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="5"/>
+    </row>
+    <row r="88" spans="2:13">
+      <c r="B88" s="4"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="5"/>
+    </row>
+    <row r="89" spans="2:13">
+      <c r="B89" s="4"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="5"/>
+    </row>
+    <row r="90" spans="2:13">
+      <c r="B90" s="4"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="5"/>
+    </row>
+    <row r="91" spans="2:13">
+      <c r="B91" s="4"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="5"/>
+    </row>
+    <row r="92" spans="2:13">
+      <c r="B92" s="4"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="5"/>
+    </row>
+    <row r="93" spans="2:13">
+      <c r="B93" s="4"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="5"/>
+    </row>
+    <row r="94" spans="2:13">
+      <c r="B94" s="4"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="5"/>
+    </row>
+    <row r="95" spans="2:13">
+      <c r="B95" s="4"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
+      <c r="M95" s="5"/>
+    </row>
+    <row r="96" spans="2:13">
+      <c r="B96" s="4"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="5"/>
+    </row>
+    <row r="97" spans="2:13">
+      <c r="B97" s="4"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+      <c r="M97" s="5"/>
+    </row>
+    <row r="98" spans="2:13">
+      <c r="B98" s="4"/>
+      <c r="C98" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="5"/>
+    </row>
+    <row r="99" spans="2:13">
+      <c r="B99" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="5"/>
+    </row>
+    <row r="100" spans="2:13">
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="9"/>
+    </row>
+    <row r="139" spans="2:14">
+      <c r="B139" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+      <c r="L139" s="2"/>
+      <c r="M139" s="2"/>
+      <c r="N139" s="3"/>
+    </row>
+    <row r="140" spans="2:14">
+      <c r="B140" s="4"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="13"/>
+      <c r="K140" s="13"/>
+      <c r="L140" s="13"/>
+      <c r="M140" s="13"/>
+      <c r="N140" s="5"/>
+    </row>
+    <row r="141" spans="2:14">
+      <c r="B141" s="4"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+      <c r="J141" s="13"/>
+      <c r="K141" s="13"/>
+      <c r="L141" s="13"/>
+      <c r="M141" s="13"/>
+      <c r="N141" s="5"/>
+    </row>
+    <row r="142" spans="2:14">
+      <c r="B142" s="4"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="13"/>
+      <c r="K142" s="13"/>
+      <c r="L142" s="13"/>
+      <c r="M142" s="13"/>
+      <c r="N142" s="5"/>
+    </row>
+    <row r="143" spans="2:14">
+      <c r="B143" s="4"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="13"/>
+      <c r="K143" s="13"/>
+      <c r="L143" s="13"/>
+      <c r="M143" s="13"/>
+      <c r="N143" s="5"/>
+    </row>
+    <row r="144" spans="2:14">
+      <c r="B144" s="4"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="13"/>
+      <c r="K144" s="13"/>
+      <c r="L144" s="13"/>
+      <c r="M144" s="13"/>
+      <c r="N144" s="5"/>
+    </row>
+    <row r="145" spans="2:14">
+      <c r="B145" s="4"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="13"/>
+      <c r="K145" s="13"/>
+      <c r="L145" s="13"/>
+      <c r="M145" s="13"/>
+      <c r="N145" s="5"/>
+    </row>
+    <row r="146" spans="2:14">
+      <c r="B146" s="4"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="13"/>
+      <c r="J146" s="13"/>
+      <c r="K146" s="13"/>
+      <c r="L146" s="13"/>
+      <c r="M146" s="13"/>
+      <c r="N146" s="5"/>
+    </row>
+    <row r="147" spans="2:14">
+      <c r="B147" s="4"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="13"/>
+      <c r="K147" s="13"/>
+      <c r="L147" s="13"/>
+      <c r="M147" s="13"/>
+      <c r="N147" s="5"/>
+    </row>
+    <row r="148" spans="2:14">
+      <c r="B148" s="4"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+      <c r="I148" s="13"/>
+      <c r="J148" s="13"/>
+      <c r="K148" s="13"/>
+      <c r="L148" s="13"/>
+      <c r="M148" s="13"/>
+      <c r="N148" s="5"/>
+    </row>
+    <row r="149" spans="2:14">
+      <c r="B149" s="4"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="13"/>
+      <c r="K149" s="13"/>
+      <c r="L149" s="13"/>
+      <c r="M149" s="13"/>
+      <c r="N149" s="5"/>
+    </row>
+    <row r="150" spans="2:14">
+      <c r="B150" s="4"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="13"/>
+      <c r="K150" s="13"/>
+      <c r="L150" s="13"/>
+      <c r="M150" s="13"/>
+      <c r="N150" s="5"/>
+    </row>
+    <row r="151" spans="2:14">
+      <c r="B151" s="4"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="13"/>
+      <c r="K151" s="13"/>
+      <c r="L151" s="13"/>
+      <c r="M151" s="13"/>
+      <c r="N151" s="5"/>
+    </row>
+    <row r="152" spans="2:14">
+      <c r="B152" s="4"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="13"/>
+      <c r="J152" s="13"/>
+      <c r="K152" s="13"/>
+      <c r="L152" s="13"/>
+      <c r="M152" s="13"/>
+      <c r="N152" s="5"/>
+    </row>
+    <row r="153" spans="2:14">
+      <c r="B153" s="4"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="13"/>
+      <c r="J153" s="13"/>
+      <c r="K153" s="13"/>
+      <c r="L153" s="13"/>
+      <c r="M153" s="13"/>
+      <c r="N153" s="5"/>
+    </row>
+    <row r="154" spans="2:14">
+      <c r="B154" s="4"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
+      <c r="I154" s="13"/>
+      <c r="J154" s="13"/>
+      <c r="K154" s="13"/>
+      <c r="L154" s="13"/>
+      <c r="M154" s="13"/>
+      <c r="N154" s="5"/>
+    </row>
+    <row r="155" spans="2:14">
+      <c r="B155" s="4"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+      <c r="G155" s="13"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="13"/>
+      <c r="J155" s="13"/>
+      <c r="K155" s="13"/>
+      <c r="L155" s="13"/>
+      <c r="M155" s="13"/>
+      <c r="N155" s="5"/>
+    </row>
+    <row r="156" spans="2:14">
+      <c r="B156" s="4"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="13"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="13"/>
+      <c r="J156" s="13"/>
+      <c r="K156" s="13"/>
+      <c r="L156" s="13"/>
+      <c r="M156" s="13"/>
+      <c r="N156" s="5"/>
+    </row>
+    <row r="157" spans="2:14">
+      <c r="B157" s="4"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="13"/>
+      <c r="G157" s="13"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="13"/>
+      <c r="J157" s="13"/>
+      <c r="K157" s="13"/>
+      <c r="L157" s="13"/>
+      <c r="M157" s="13"/>
+      <c r="N157" s="5"/>
+    </row>
+    <row r="158" spans="2:14">
+      <c r="B158" s="4"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="13"/>
+      <c r="K158" s="13"/>
+      <c r="L158" s="13"/>
+      <c r="M158" s="13"/>
+      <c r="N158" s="5"/>
+    </row>
+    <row r="159" spans="2:14">
+      <c r="B159" s="4"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="13"/>
+      <c r="J159" s="13"/>
+      <c r="K159" s="13"/>
+      <c r="L159" s="13"/>
+      <c r="M159" s="13"/>
+      <c r="N159" s="5"/>
+    </row>
+    <row r="160" spans="2:14">
+      <c r="B160" s="4"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="13"/>
+      <c r="K160" s="13"/>
+      <c r="L160" s="13"/>
+      <c r="M160" s="13"/>
+      <c r="N160" s="5"/>
+    </row>
+    <row r="161" spans="2:14">
+      <c r="B161" s="4"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="13"/>
+      <c r="K161" s="13"/>
+      <c r="L161" s="13"/>
+      <c r="M161" s="13"/>
+      <c r="N161" s="5"/>
+    </row>
+    <row r="162" spans="2:14">
+      <c r="B162" s="4"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="13"/>
+      <c r="I162" s="13"/>
+      <c r="J162" s="13"/>
+      <c r="K162" s="13"/>
+      <c r="L162" s="13"/>
+      <c r="M162" s="13"/>
+      <c r="N162" s="5"/>
+    </row>
+    <row r="163" spans="2:14">
+      <c r="B163" s="4"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="13"/>
+      <c r="J163" s="13"/>
+      <c r="K163" s="13"/>
+      <c r="L163" s="13"/>
+      <c r="M163" s="13"/>
+      <c r="N163" s="5"/>
+    </row>
+    <row r="164" spans="2:14">
+      <c r="B164" s="4"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="13"/>
+      <c r="J164" s="13"/>
+      <c r="K164" s="13"/>
+      <c r="L164" s="13"/>
+      <c r="M164" s="13"/>
+      <c r="N164" s="5"/>
+    </row>
+    <row r="165" spans="2:14">
+      <c r="B165" s="4"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="13"/>
+      <c r="J165" s="13"/>
+      <c r="K165" s="13"/>
+      <c r="L165" s="13"/>
+      <c r="M165" s="13"/>
+      <c r="N165" s="5"/>
+    </row>
+    <row r="166" spans="2:14">
+      <c r="B166" s="4"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="13"/>
+      <c r="J166" s="13"/>
+      <c r="K166" s="13"/>
+      <c r="L166" s="13"/>
+      <c r="M166" s="13"/>
+      <c r="N166" s="5"/>
+    </row>
+    <row r="167" spans="2:14">
+      <c r="B167" s="4"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="13"/>
+      <c r="J167" s="13"/>
+      <c r="K167" s="13"/>
+      <c r="L167" s="13"/>
+      <c r="M167" s="13"/>
+      <c r="N167" s="5"/>
+    </row>
+    <row r="168" spans="2:14">
+      <c r="B168" s="4"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="13"/>
+      <c r="J168" s="13"/>
+      <c r="K168" s="13"/>
+      <c r="L168" s="13"/>
+      <c r="M168" s="13"/>
+      <c r="N168" s="5"/>
+    </row>
+    <row r="169" spans="2:14">
+      <c r="B169" s="4"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="13"/>
+      <c r="J169" s="13"/>
+      <c r="K169" s="13"/>
+      <c r="L169" s="13"/>
+      <c r="M169" s="13"/>
+      <c r="N169" s="5"/>
+    </row>
+    <row r="170" spans="2:14">
+      <c r="B170" s="4"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="13"/>
+      <c r="J170" s="13"/>
+      <c r="K170" s="13"/>
+      <c r="L170" s="13"/>
+      <c r="M170" s="13"/>
+      <c r="N170" s="5"/>
+    </row>
+    <row r="171" spans="2:14">
+      <c r="B171" s="7"/>
+      <c r="C171" s="8"/>
+      <c r="D171" s="8"/>
+      <c r="E171" s="8"/>
+      <c r="F171" s="8"/>
+      <c r="G171" s="8"/>
+      <c r="H171" s="8"/>
+      <c r="I171" s="8"/>
+      <c r="J171" s="8"/>
+      <c r="K171" s="8"/>
+      <c r="L171" s="8"/>
+      <c r="M171" s="8"/>
+      <c r="N171" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>